<commit_message>
added remaining one-vs-one decision values files.
</commit_message>
<xml_diff>
--- a/custom/multi-class bottleneck/data/decision_values_one-vs-one-N-200-Imprint..xlsx
+++ b/custom/multi-class bottleneck/data/decision_values_one-vs-one-N-200-Imprint..xlsx
@@ -1267,6 +1267,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1282,8 +1284,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1631,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AK1:AS1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1:AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,30 +1642,32 @@
     <col min="3" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="19" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" style="3" customWidth="1"/>
-    <col min="27" max="27" width="12.85546875" style="4" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" customWidth="1"/>
-    <col min="31" max="31" width="12.42578125" customWidth="1"/>
-    <col min="32" max="32" width="12.85546875" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" customWidth="1"/>
-    <col min="35" max="35" width="15.85546875" customWidth="1"/>
-    <col min="36" max="36" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="15.85546875" hidden="1" customWidth="1"/>
+    <col min="15" max="19" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="15.85546875" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="12.7109375" customWidth="1"/>
     <col min="38" max="38" width="11.5703125" customWidth="1"/>
-    <col min="39" max="45" width="9.140625" customWidth="1"/>
+    <col min="39" max="43" width="9.140625" customWidth="1"/>
+    <col min="44" max="44" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" customWidth="1"/>
     <col min="46" max="46" width="13.5703125" customWidth="1"/>
     <col min="47" max="47" width="11.85546875" customWidth="1"/>
     <col min="48" max="52" width="9.140625" customWidth="1"/>
@@ -1674,82 +1676,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="11" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="6" t="s">
         <v>236</v>
       </c>
       <c r="N1" s="5">
         <f>(SUM(N3:N202)/COUNT(N3:N202))*100</f>
         <v>26</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="U1" s="12">
+      <c r="U1" s="7">
         <f>(SUM(U3:U202)/COUNT(U3:U202))*100</f>
         <v>18</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="8" t="s">
+      <c r="W1" s="11"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="6" t="s">
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6" t="s">
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
       <c r="AH1" t="s">
         <v>230</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="AJ1" s="12">
+      <c r="AJ1" s="7">
         <f>(SUM(AJ3:AJ202)/COUNT(AJ3:AJ202))*100</f>
         <v>16.5</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="AL1" s="6"/>
-      <c r="AR1" s="12" t="s">
+      <c r="AL1" s="8"/>
+      <c r="AR1" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="AS1" s="12">
+      <c r="AS1" s="7">
         <f>(SUM(AS3:AS202)/COUNT(AS3:AS202))*100</f>
         <v>28.499999999999996</v>
       </c>
       <c r="AT1" t="s">
         <v>235</v>
       </c>
-      <c r="BA1" s="12" t="s">
+      <c r="BA1" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="BB1" s="12">
+      <c r="BB1" s="7">
         <f>(SUM(BB3:BB202)/COUNT(BB3:BB202))*100</f>
         <v>13</v>
       </c>

</xml_diff>